<commit_message>
add schema with _GIT_METADATA; make data based on this schema
</commit_message>
<xml_diff>
--- a/tests/fixtures/bad_data_file.xlsx
+++ b/tests/fixtures/bad_data_file.xlsx
@@ -90,7 +90,35 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
+          <t>Enter a string.
+Value must be less than or equal to 255 characters.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A6" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
           <t>Enter a comma-separated list of values from "References:A" or blank.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Enter a string.
+Value must be less than or equal to 255 characters.</t>
         </r>
       </text>
     </comment>
@@ -139,7 +167,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Id</t>
   </si>
@@ -159,7 +187,7 @@
     <t>Revision</t>
   </si>
   <si>
-    <t>aed822c5523c0b93f85024d3678303c57c2e0cd4</t>
+    <t>9606a6c0b62d3f3e3dfbb905a965ecb808d2365b</t>
   </si>
   <si>
     <t>Existing attr</t>
@@ -168,10 +196,22 @@
     <t>x</t>
   </si>
   <si>
+    <t>Branch</t>
+  </si>
+  <si>
+    <t>master</t>
+  </si>
+  <si>
     <t>References</t>
   </si>
   <si>
     <t>ref_1, ref_2</t>
+  </si>
+  <si>
+    <t>Url</t>
+  </si>
+  <si>
+    <t>https://github.com/KarrLab/test_repo.git</t>
   </si>
   <si>
     <t>Value</t>
@@ -551,7 +591,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
@@ -619,9 +659,31 @@
         <v>10</v>
       </c>
     </row>
+    <row r="6" spans="1:3" ht="15.01" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="15.01" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1" insertRows="0" deleteRows="0" sort="0" autoFilter="0"/>
-  <dataValidations count="5">
+  <dataValidations count="7">
     <dataValidation type="textLength" errorStyle="warning" showInputMessage="1" showErrorMessage="1" errorTitle="Id" error="Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long&#10;&#10;Value must be a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." promptTitle="Id" prompt="Enter a unique string identifier that (1) starts with a letter, (2) is composed of letters, numbers and underscores, and (3) is less than 64 characters long&#10;&#10;Enter a string.&#10;&#10;Value must be between 1 and 63 characters.&#10;&#10;Value must be unique." sqref="B1:C1">
       <formula1>1</formula1>
       <formula2>63</formula2>
@@ -635,7 +697,13 @@
     <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Existing attr" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Existing attr" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B4:C4">
       <formula1>255</formula1>
     </dataValidation>
-    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="B5:C5"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Branch" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Branch" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B5:C5">
+      <formula1>255</formula1>
+    </dataValidation>
+    <dataValidation errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="References" error="Value must be a comma-separated list of values from &quot;References:A&quot; or blank." promptTitle="References" prompt="Enter a comma-separated list of values from &quot;References:A&quot; or blank." sqref="B6:C6"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Url" error="Value must be a string.&#10;&#10;Value must be less than or equal to 255 characters." promptTitle="Url" prompt="Enter a string.&#10;&#10;Value must be less than or equal to 255 characters." sqref="B7:C7">
+      <formula1>255</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -662,23 +730,23 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="15.01" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.01" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>